<commit_message>
add naming of own so's
</commit_message>
<xml_diff>
--- a/sheet_template.xlsx
+++ b/sheet_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\GitHub\klub-100-maker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E3BCC0-2631-4423-B4F5-C117E3084251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA571EE-C46F-4EA0-B970-EBC5E0E40E47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,10 +414,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.38671875" defaultRowHeight="15.75" customHeight="1"/>
@@ -426,9 +426,10 @@
     <col min="2" max="2" width="46.6640625" customWidth="1"/>
     <col min="3" max="4" width="19.5" customWidth="1"/>
     <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="24.0546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -444,373 +445,401 @@
       <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="6"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="7"/>
       <c r="B3" s="5"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="6"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="7"/>
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" s="5"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" s="5"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="5"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="5"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="22" spans="1:6" ht="12.3">
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" ht="12.3">
       <c r="A22" s="1"/>
       <c r="B22" s="5"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" ht="12.3">
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" ht="12.3">
       <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" ht="12.3">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" ht="12.3">
       <c r="A24" s="1"/>
       <c r="B24" s="5"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:6" ht="12.3">
+    <row r="25" spans="1:7" ht="12.3">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" ht="12.3">
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" ht="12.3">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" ht="12.3">
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="12.3">
       <c r="A27" s="1"/>
       <c r="B27" s="5"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="13.8">
+    <row r="28" spans="1:7" ht="13.8">
       <c r="A28" s="8"/>
       <c r="B28" s="5"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:6" ht="12.3">
+    <row r="29" spans="1:7" ht="12.3">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:6" ht="12.3">
+    <row r="30" spans="1:7" ht="12.3">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:6" ht="12.3">
+    <row r="31" spans="1:7" ht="12.3">
       <c r="A31" s="7"/>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:6" ht="12.3">
+    <row r="32" spans="1:7" ht="12.3">
       <c r="A32" s="7"/>
       <c r="B32" s="6"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:6" ht="12.3">
+    <row r="33" spans="1:7" ht="12.3">
       <c r="A33" s="1"/>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:6" ht="12.3">
+    <row r="34" spans="1:7" ht="12.3">
       <c r="A34" s="1"/>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:6" ht="12.3">
+    <row r="35" spans="1:7" ht="12.3">
       <c r="A35" s="1"/>
       <c r="B35" s="5"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:6" ht="12.3">
+    <row r="36" spans="1:7" ht="12.3">
       <c r="A36" s="1"/>
       <c r="B36" s="5"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:6" ht="12.3">
+    <row r="37" spans="1:7" ht="12.3">
       <c r="A37" s="1"/>
       <c r="B37" s="6"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:6" ht="12.3">
+    <row r="38" spans="1:7" ht="12.3">
       <c r="A38" s="1"/>
       <c r="B38" s="5"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:6" ht="12.3">
+    <row r="39" spans="1:7" ht="12.3">
       <c r="A39" s="7"/>
       <c r="B39" s="5"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:6" ht="12.3">
+    <row r="40" spans="1:7" ht="12.3">
       <c r="A40" s="1"/>
       <c r="B40" s="5"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:6" ht="12.3">
+    <row r="41" spans="1:7" ht="12.3">
       <c r="A41" s="1"/>
       <c r="B41" s="5"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" ht="12.3">
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" ht="12.3">
       <c r="A42" s="1"/>
       <c r="B42" s="5"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" ht="12.3">
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" ht="12.3">
       <c r="A43" s="1"/>
       <c r="B43" s="5"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:6" ht="12.3">
+    <row r="44" spans="1:7" ht="12.3">
       <c r="A44" s="1"/>
       <c r="B44" s="5"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:6" ht="12.3">
+    <row r="45" spans="1:7" ht="12.3">
       <c r="A45" s="7"/>
       <c r="B45" s="5"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" ht="12.3">
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" ht="12.3">
       <c r="A46" s="7"/>
       <c r="B46" s="6"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:6" ht="12.3">
+    <row r="47" spans="1:7" ht="12.3">
       <c r="A47" s="1"/>
       <c r="B47" s="5"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:6" ht="12.3">
+    <row r="48" spans="1:7" ht="12.3">
       <c r="A48" s="1"/>
       <c r="B48" s="5"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:6" ht="12.3">
+    <row r="49" spans="1:7" ht="12.3">
       <c r="A49" s="1"/>
       <c r="B49" s="5"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:6" ht="12.3">
+    <row r="50" spans="1:7" ht="12.3">
       <c r="A50" s="1"/>
       <c r="B50" s="6"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:6" ht="12.3">
+    <row r="51" spans="1:7" ht="12.3">
       <c r="A51" s="1"/>
       <c r="B51" s="6"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:6" ht="12.3">
+    <row r="52" spans="1:7" ht="12.3">
       <c r="A52" s="1"/>
       <c r="B52" s="5"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:6" ht="12.3">
+    <row r="53" spans="1:7" ht="12.3">
       <c r="A53" s="1"/>
       <c r="B53" s="5"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:6" ht="12.3">
+    <row r="54" spans="1:7" ht="12.3">
       <c r="A54" s="1"/>
       <c r="B54" s="5"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="56" spans="1:6" ht="12.3">
+    <row r="56" spans="1:7" ht="12.3">
       <c r="A56" s="7"/>
       <c r="B56" s="5"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" ht="12.3">
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" ht="12.3">
       <c r="A57" s="1"/>
       <c r="B57" s="5"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:6" ht="12.3">
+    <row r="58" spans="1:7" ht="12.3">
       <c r="A58" s="1"/>
       <c r="B58" s="5"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:6" ht="12.3">
+    <row r="59" spans="1:7" ht="12.3">
       <c r="A59" s="1"/>
       <c r="B59" s="5"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:6" ht="12.3">
+    <row r="60" spans="1:7" ht="12.3">
       <c r="A60" s="7"/>
       <c r="B60" s="6"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:6" ht="12.3">
+    <row r="61" spans="1:7" ht="12.3">
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:6" ht="12.3">
+    <row r="62" spans="1:7" ht="12.3">
       <c r="A62" s="1"/>
       <c r="B62" s="5"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:6" ht="12.3">
+    <row r="63" spans="1:7" ht="12.3">
       <c r="A63" s="1"/>
       <c r="B63" s="5"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:6" ht="12.3">
+    <row r="64" spans="1:7" ht="12.3">
       <c r="A64" s="1"/>
       <c r="B64" s="5"/>
       <c r="C64" s="1"/>
@@ -988,85 +1017,85 @@
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
-    <row r="98" spans="1:6" ht="12.3">
+    <row r="98" spans="1:7" ht="12.3">
       <c r="A98" s="1"/>
       <c r="B98" s="5"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="1:6" ht="12.3">
+    <row r="99" spans="1:7" ht="12.3">
       <c r="A99" s="1"/>
       <c r="B99" s="5"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="1:6" ht="12.3">
+    <row r="100" spans="1:7" ht="12.3">
       <c r="A100" s="1"/>
       <c r="B100" s="6"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
-    <row r="101" spans="1:6" ht="12.3">
+    <row r="101" spans="1:7" ht="12.3">
       <c r="A101" s="1"/>
       <c r="B101" s="5"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-    </row>
-    <row r="103" spans="1:6" ht="12.3">
+      <c r="G101" s="1"/>
+    </row>
+    <row r="103" spans="1:7" ht="12.3">
       <c r="A103" s="2"/>
     </row>
-    <row r="104" spans="1:6" ht="12.3">
+    <row r="104" spans="1:7" ht="12.3">
       <c r="A104" s="1"/>
       <c r="B104" s="6"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:6" ht="12.3">
+    <row r="105" spans="1:7" ht="12.3">
       <c r="A105" s="1"/>
       <c r="B105" s="5"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
-      <c r="F105" s="1"/>
-    </row>
-    <row r="106" spans="1:6" ht="12.3">
+      <c r="G105" s="1"/>
+    </row>
+    <row r="106" spans="1:7" ht="12.3">
       <c r="A106" s="1"/>
       <c r="B106" s="6"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="1:6" ht="12.3">
+    <row r="107" spans="1:7" ht="12.3">
       <c r="A107" s="7"/>
       <c r="B107" s="5"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
     </row>
-    <row r="108" spans="1:6" ht="12.3">
+    <row r="108" spans="1:7" ht="12.3">
       <c r="A108" s="1"/>
       <c r="B108" s="6"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
-    <row r="109" spans="1:6" ht="12.3">
+    <row r="109" spans="1:7" ht="12.3">
       <c r="A109" s="1"/>
       <c r="B109" s="5"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
-    <row r="110" spans="1:6" ht="12.3">
+    <row r="110" spans="1:7" ht="12.3">
       <c r="A110" s="1"/>
       <c r="B110" s="5"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="1:6" ht="12.3">
+    <row r="111" spans="1:7" ht="12.3">
       <c r="A111" s="1"/>
       <c r="B111" s="6"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="1:6" ht="12.3">
+    <row r="112" spans="1:7" ht="12.3">
       <c r="A112" s="7"/>
       <c r="B112" s="6"/>
       <c r="C112" s="1"/>
@@ -1130,10 +1159,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.38671875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1141,10 +1170,10 @@
     <col min="1" max="1" width="42.88671875" customWidth="1"/>
     <col min="2" max="2" width="53.38671875" customWidth="1"/>
     <col min="3" max="3" width="23.0546875" customWidth="1"/>
-    <col min="4" max="5" width="24.0546875" customWidth="1"/>
+    <col min="4" max="4" width="24.0546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1157,173 +1186,149 @@
       <c r="D1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="5"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="6"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="5"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="5"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" s="1"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="5"/>
       <c r="C17" s="1"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="5"/>
       <c r="C18" s="4"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="5"/>
       <c r="C19" s="4"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="5"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="5"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="12.3">
+    </row>
+    <row r="22" spans="1:4" ht="12.3">
       <c r="A22" s="1"/>
       <c r="B22" s="5"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="12.3">
+    </row>
+    <row r="23" spans="1:4" ht="12.3">
       <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="12.3">
+    </row>
+    <row r="24" spans="1:4" ht="12.3">
       <c r="A24" s="1"/>
       <c r="B24" s="5"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:5" ht="12.3">
+    <row r="25" spans="1:4" ht="12.3">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" ht="12.3">
+    </row>
+    <row r="26" spans="1:4" ht="12.3">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" ht="12.3">
+    </row>
+    <row r="27" spans="1:4" ht="12.3">
       <c r="A27" s="1"/>
       <c r="B27" s="5"/>
       <c r="C27" s="1"/>

</xml_diff>